<commit_message>
Added more functionalites in streamlite
</commit_message>
<xml_diff>
--- a/paragon_data_combined.xlsx
+++ b/paragon_data_combined.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:P26"/>
+  <dimension ref="A1:P13"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -1205,732 +1205,6 @@
         <v>28.9</v>
       </c>
     </row>
-    <row r="14">
-      <c r="A14" t="inlineStr">
-        <is>
-          <t>2024-10-10</t>
-        </is>
-      </c>
-      <c r="B14" t="inlineStr">
-        <is>
-          <t>10:20:45</t>
-        </is>
-      </c>
-      <c r="C14" t="inlineStr">
-        <is>
-          <t>WodaGaz Muszy1,5l        A</t>
-        </is>
-      </c>
-      <c r="D14" t="inlineStr">
-        <is>
-          <t>A</t>
-        </is>
-      </c>
-      <c r="E14" t="n">
-        <v>289</v>
-      </c>
-      <c r="F14" t="n">
-        <v>1734</v>
-      </c>
-      <c r="G14" t="inlineStr">
-        <is>
-          <t>6</t>
-        </is>
-      </c>
-      <c r="H14" t="inlineStr"/>
-      <c r="I14" t="inlineStr"/>
-      <c r="J14" t="inlineStr"/>
-      <c r="K14" t="inlineStr"/>
-      <c r="L14" t="inlineStr">
-        <is>
-          <t>Woda Gaz Muszy 1,5l</t>
-        </is>
-      </c>
-      <c r="M14" t="n">
-        <v>1.5</v>
-      </c>
-      <c r="N14" t="inlineStr">
-        <is>
-          <t>l</t>
-        </is>
-      </c>
-      <c r="O14" t="n">
-        <v>1734</v>
-      </c>
-      <c r="P14" t="n">
-        <v>17.34</v>
-      </c>
-    </row>
-    <row r="15">
-      <c r="A15" t="inlineStr">
-        <is>
-          <t>2024-10-10</t>
-        </is>
-      </c>
-      <c r="B15" t="inlineStr">
-        <is>
-          <t>10:20:45</t>
-        </is>
-      </c>
-      <c r="C15" t="inlineStr">
-        <is>
-          <t>SerekProt.Malina200g     C</t>
-        </is>
-      </c>
-      <c r="D15" t="inlineStr">
-        <is>
-          <t>C</t>
-        </is>
-      </c>
-      <c r="E15" t="n">
-        <v>335</v>
-      </c>
-      <c r="F15" t="n">
-        <v>335</v>
-      </c>
-      <c r="G15" t="inlineStr">
-        <is>
-          <t>1</t>
-        </is>
-      </c>
-      <c r="H15" t="inlineStr"/>
-      <c r="I15" t="inlineStr"/>
-      <c r="J15" t="inlineStr"/>
-      <c r="K15" t="inlineStr"/>
-      <c r="L15" t="inlineStr">
-        <is>
-          <t>Serek Prot. Malina 200g</t>
-        </is>
-      </c>
-      <c r="M15" t="n">
-        <v>200</v>
-      </c>
-      <c r="N15" t="inlineStr">
-        <is>
-          <t>g</t>
-        </is>
-      </c>
-      <c r="O15" t="n">
-        <v>335</v>
-      </c>
-      <c r="P15" t="n">
-        <v>3.35</v>
-      </c>
-    </row>
-    <row r="16">
-      <c r="A16" t="inlineStr">
-        <is>
-          <t>2024-10-11</t>
-        </is>
-      </c>
-      <c r="B16" t="inlineStr">
-        <is>
-          <t>16:58:42</t>
-        </is>
-      </c>
-      <c r="C16" t="inlineStr">
-        <is>
-          <t>PiwoPer0 0,5lB BZW       A</t>
-        </is>
-      </c>
-      <c r="D16" t="inlineStr">
-        <is>
-          <t>A</t>
-        </is>
-      </c>
-      <c r="E16" t="n">
-        <v>269</v>
-      </c>
-      <c r="F16" t="n">
-        <v>1614</v>
-      </c>
-      <c r="G16" t="inlineStr">
-        <is>
-          <t>6</t>
-        </is>
-      </c>
-      <c r="H16" t="inlineStr"/>
-      <c r="I16" t="inlineStr"/>
-      <c r="J16" t="inlineStr"/>
-      <c r="K16" t="inlineStr"/>
-      <c r="L16" t="inlineStr">
-        <is>
-          <t>Piwo Per 0 0,5l B BZW</t>
-        </is>
-      </c>
-      <c r="M16" t="n">
-        <v>0.5</v>
-      </c>
-      <c r="N16" t="inlineStr">
-        <is>
-          <t>l</t>
-        </is>
-      </c>
-      <c r="O16" t="n">
-        <v>1614</v>
-      </c>
-      <c r="P16" t="n">
-        <v>16.14</v>
-      </c>
-    </row>
-    <row r="17">
-      <c r="A17" t="inlineStr">
-        <is>
-          <t>2024-10-11</t>
-        </is>
-      </c>
-      <c r="B17" t="inlineStr">
-        <is>
-          <t>16:58:42</t>
-        </is>
-      </c>
-      <c r="C17" t="inlineStr">
-        <is>
-          <t>NerkoMigdałTop150g       C</t>
-        </is>
-      </c>
-      <c r="D17" t="inlineStr">
-        <is>
-          <t>C</t>
-        </is>
-      </c>
-      <c r="E17" t="n">
-        <v>899</v>
-      </c>
-      <c r="F17" t="n">
-        <v>899</v>
-      </c>
-      <c r="G17" t="inlineStr">
-        <is>
-          <t>1</t>
-        </is>
-      </c>
-      <c r="H17" t="inlineStr"/>
-      <c r="I17" t="inlineStr"/>
-      <c r="J17" t="inlineStr"/>
-      <c r="K17" t="inlineStr"/>
-      <c r="L17" t="inlineStr">
-        <is>
-          <t>Nerko Migdał Top 150g</t>
-        </is>
-      </c>
-      <c r="M17" t="n">
-        <v>150</v>
-      </c>
-      <c r="N17" t="inlineStr">
-        <is>
-          <t>g</t>
-        </is>
-      </c>
-      <c r="O17" t="n">
-        <v>899</v>
-      </c>
-      <c r="P17" t="n">
-        <v>8.99</v>
-      </c>
-    </row>
-    <row r="18">
-      <c r="A18" t="inlineStr">
-        <is>
-          <t>2024-10-11</t>
-        </is>
-      </c>
-      <c r="B18" t="inlineStr">
-        <is>
-          <t>16:58:42</t>
-        </is>
-      </c>
-      <c r="C18" t="inlineStr">
-        <is>
-          <t>Kieł.śląs/biał270g       C</t>
-        </is>
-      </c>
-      <c r="D18" t="inlineStr">
-        <is>
-          <t>C</t>
-        </is>
-      </c>
-      <c r="E18" t="n">
-        <v>999</v>
-      </c>
-      <c r="F18" t="n">
-        <v>999</v>
-      </c>
-      <c r="G18" t="inlineStr">
-        <is>
-          <t>1</t>
-        </is>
-      </c>
-      <c r="H18" t="inlineStr"/>
-      <c r="I18" t="inlineStr"/>
-      <c r="J18" t="inlineStr"/>
-      <c r="K18" t="inlineStr"/>
-      <c r="L18" t="inlineStr">
-        <is>
-          <t>Kieł śląs/biał 270g</t>
-        </is>
-      </c>
-      <c r="M18" t="n">
-        <v>270</v>
-      </c>
-      <c r="N18" t="inlineStr">
-        <is>
-          <t>g</t>
-        </is>
-      </c>
-      <c r="O18" t="n">
-        <v>999</v>
-      </c>
-      <c r="P18" t="n">
-        <v>9.99</v>
-      </c>
-    </row>
-    <row r="19">
-      <c r="A19" t="inlineStr">
-        <is>
-          <t>2024-10-11</t>
-        </is>
-      </c>
-      <c r="B19" t="inlineStr">
-        <is>
-          <t>16:58:42</t>
-        </is>
-      </c>
-      <c r="C19" t="inlineStr">
-        <is>
-          <t>PierogiRuskie800g        C</t>
-        </is>
-      </c>
-      <c r="D19" t="inlineStr">
-        <is>
-          <t>C</t>
-        </is>
-      </c>
-      <c r="E19" t="n">
-        <v>725</v>
-      </c>
-      <c r="F19" t="n">
-        <v>1450</v>
-      </c>
-      <c r="G19" t="inlineStr">
-        <is>
-          <t>2</t>
-        </is>
-      </c>
-      <c r="H19" t="n">
-        <v>1450</v>
-      </c>
-      <c r="I19" t="n">
-        <v>252</v>
-      </c>
-      <c r="J19" t="b">
-        <v>1</v>
-      </c>
-      <c r="K19" t="b">
-        <v>0</v>
-      </c>
-      <c r="L19" t="inlineStr">
-        <is>
-          <t>Pierogi Ruskie 800g</t>
-        </is>
-      </c>
-      <c r="M19" t="n">
-        <v>800</v>
-      </c>
-      <c r="N19" t="inlineStr">
-        <is>
-          <t>g</t>
-        </is>
-      </c>
-      <c r="O19" t="n">
-        <v>1198</v>
-      </c>
-      <c r="P19" t="n">
-        <v>11.98</v>
-      </c>
-    </row>
-    <row r="20">
-      <c r="A20" t="inlineStr">
-        <is>
-          <t>2024-10-11</t>
-        </is>
-      </c>
-      <c r="B20" t="inlineStr">
-        <is>
-          <t>16:58:42</t>
-        </is>
-      </c>
-      <c r="C20" t="inlineStr">
-        <is>
-          <t>FasolaŻół Ziel450g       C</t>
-        </is>
-      </c>
-      <c r="D20" t="inlineStr">
-        <is>
-          <t>C</t>
-        </is>
-      </c>
-      <c r="E20" t="n">
-        <v>599</v>
-      </c>
-      <c r="F20" t="n">
-        <v>1198</v>
-      </c>
-      <c r="G20" t="inlineStr">
-        <is>
-          <t>2</t>
-        </is>
-      </c>
-      <c r="H20" t="n">
-        <v>1198</v>
-      </c>
-      <c r="I20" t="n">
-        <v>200</v>
-      </c>
-      <c r="J20" t="b">
-        <v>1</v>
-      </c>
-      <c r="K20" t="b">
-        <v>0</v>
-      </c>
-      <c r="L20" t="inlineStr">
-        <is>
-          <t>Fasola Żół Ziel 450g</t>
-        </is>
-      </c>
-      <c r="M20" t="n">
-        <v>450</v>
-      </c>
-      <c r="N20" t="inlineStr">
-        <is>
-          <t>g</t>
-        </is>
-      </c>
-      <c r="O20" t="n">
-        <v>998</v>
-      </c>
-      <c r="P20" t="n">
-        <v>9.98</v>
-      </c>
-    </row>
-    <row r="21">
-      <c r="A21" t="inlineStr">
-        <is>
-          <t>2024-10-11</t>
-        </is>
-      </c>
-      <c r="B21" t="inlineStr">
-        <is>
-          <t>16:58:42</t>
-        </is>
-      </c>
-      <c r="C21" t="inlineStr">
-        <is>
-          <t>KiełbasaChorizo280g      C</t>
-        </is>
-      </c>
-      <c r="D21" t="inlineStr">
-        <is>
-          <t>C</t>
-        </is>
-      </c>
-      <c r="E21" t="n">
-        <v>1599</v>
-      </c>
-      <c r="F21" t="n">
-        <v>1599</v>
-      </c>
-      <c r="G21" t="inlineStr">
-        <is>
-          <t>1</t>
-        </is>
-      </c>
-      <c r="H21" t="inlineStr"/>
-      <c r="I21" t="inlineStr"/>
-      <c r="J21" t="inlineStr"/>
-      <c r="K21" t="inlineStr"/>
-      <c r="L21" t="inlineStr">
-        <is>
-          <t>Kiełbasa Chorizo 280g</t>
-        </is>
-      </c>
-      <c r="M21" t="n">
-        <v>280</v>
-      </c>
-      <c r="N21" t="inlineStr">
-        <is>
-          <t>g</t>
-        </is>
-      </c>
-      <c r="O21" t="n">
-        <v>1599</v>
-      </c>
-      <c r="P21" t="n">
-        <v>15.99</v>
-      </c>
-    </row>
-    <row r="22">
-      <c r="A22" t="inlineStr">
-        <is>
-          <t>2024-10-11</t>
-        </is>
-      </c>
-      <c r="B22" t="inlineStr">
-        <is>
-          <t>16:58:42</t>
-        </is>
-      </c>
-      <c r="C22" t="inlineStr">
-        <is>
-          <t>BWę/ParMorlin150 g       C</t>
-        </is>
-      </c>
-      <c r="D22" t="inlineStr">
-        <is>
-          <t>C</t>
-        </is>
-      </c>
-      <c r="E22" t="n">
-        <v>759</v>
-      </c>
-      <c r="F22" t="n">
-        <v>1518</v>
-      </c>
-      <c r="G22" t="inlineStr">
-        <is>
-          <t>2</t>
-        </is>
-      </c>
-      <c r="H22" t="inlineStr"/>
-      <c r="I22" t="inlineStr"/>
-      <c r="J22" t="inlineStr"/>
-      <c r="K22" t="inlineStr"/>
-      <c r="L22" t="inlineStr">
-        <is>
-          <t>BWę/ Par Morlin 150 g</t>
-        </is>
-      </c>
-      <c r="M22" t="inlineStr"/>
-      <c r="N22" t="inlineStr"/>
-      <c r="O22" t="n">
-        <v>1518</v>
-      </c>
-      <c r="P22" t="n">
-        <v>15.18</v>
-      </c>
-    </row>
-    <row r="23">
-      <c r="A23" t="inlineStr">
-        <is>
-          <t>2024-10-11</t>
-        </is>
-      </c>
-      <c r="B23" t="inlineStr">
-        <is>
-          <t>16:58:42</t>
-        </is>
-      </c>
-      <c r="C23" t="inlineStr">
-        <is>
-          <t>Ser Edamski 250g         C</t>
-        </is>
-      </c>
-      <c r="D23" t="inlineStr">
-        <is>
-          <t>C</t>
-        </is>
-      </c>
-      <c r="E23" t="n">
-        <v>849</v>
-      </c>
-      <c r="F23" t="n">
-        <v>1698</v>
-      </c>
-      <c r="G23" t="inlineStr">
-        <is>
-          <t>2</t>
-        </is>
-      </c>
-      <c r="H23" t="inlineStr"/>
-      <c r="I23" t="inlineStr"/>
-      <c r="J23" t="inlineStr"/>
-      <c r="K23" t="inlineStr"/>
-      <c r="L23" t="inlineStr">
-        <is>
-          <t>Ser Edamski 250g</t>
-        </is>
-      </c>
-      <c r="M23" t="n">
-        <v>250</v>
-      </c>
-      <c r="N23" t="inlineStr">
-        <is>
-          <t>g</t>
-        </is>
-      </c>
-      <c r="O23" t="n">
-        <v>1698</v>
-      </c>
-      <c r="P23" t="n">
-        <v>16.98</v>
-      </c>
-    </row>
-    <row r="24">
-      <c r="A24" t="inlineStr">
-        <is>
-          <t>2024-10-11</t>
-        </is>
-      </c>
-      <c r="B24" t="inlineStr">
-        <is>
-          <t>16:58:42</t>
-        </is>
-      </c>
-      <c r="C24" t="inlineStr">
-        <is>
-          <t>Serek z palusz  35g      C</t>
-        </is>
-      </c>
-      <c r="D24" t="inlineStr">
-        <is>
-          <t>C</t>
-        </is>
-      </c>
-      <c r="E24" t="n">
-        <v>299</v>
-      </c>
-      <c r="F24" t="n">
-        <v>299</v>
-      </c>
-      <c r="G24" t="inlineStr">
-        <is>
-          <t>1</t>
-        </is>
-      </c>
-      <c r="H24" t="inlineStr"/>
-      <c r="I24" t="inlineStr"/>
-      <c r="J24" t="inlineStr"/>
-      <c r="K24" t="inlineStr"/>
-      <c r="L24" t="inlineStr">
-        <is>
-          <t>Serek z palusz 35g</t>
-        </is>
-      </c>
-      <c r="M24" t="n">
-        <v>35</v>
-      </c>
-      <c r="N24" t="inlineStr">
-        <is>
-          <t>g</t>
-        </is>
-      </c>
-      <c r="O24" t="n">
-        <v>299</v>
-      </c>
-      <c r="P24" t="n">
-        <v>2.99</v>
-      </c>
-    </row>
-    <row r="25">
-      <c r="A25" t="inlineStr">
-        <is>
-          <t>2024-10-11</t>
-        </is>
-      </c>
-      <c r="B25" t="inlineStr">
-        <is>
-          <t>16:58:42</t>
-        </is>
-      </c>
-      <c r="C25" t="inlineStr">
-        <is>
-          <t>MiętaKolendraXLVF        C</t>
-        </is>
-      </c>
-      <c r="D25" t="inlineStr">
-        <is>
-          <t>C</t>
-        </is>
-      </c>
-      <c r="E25" t="n">
-        <v>799</v>
-      </c>
-      <c r="F25" t="n">
-        <v>799</v>
-      </c>
-      <c r="G25" t="inlineStr">
-        <is>
-          <t>1</t>
-        </is>
-      </c>
-      <c r="H25" t="inlineStr"/>
-      <c r="I25" t="inlineStr"/>
-      <c r="J25" t="inlineStr"/>
-      <c r="K25" t="inlineStr"/>
-      <c r="L25" t="inlineStr">
-        <is>
-          <t>Mięta Kolendra XLVF</t>
-        </is>
-      </c>
-      <c r="M25" t="inlineStr"/>
-      <c r="N25" t="inlineStr"/>
-      <c r="O25" t="n">
-        <v>799</v>
-      </c>
-      <c r="P25" t="n">
-        <v>7.99</v>
-      </c>
-    </row>
-    <row r="26">
-      <c r="A26" t="inlineStr">
-        <is>
-          <t>2024-10-11</t>
-        </is>
-      </c>
-      <c r="B26" t="inlineStr">
-        <is>
-          <t>16:58:42</t>
-        </is>
-      </c>
-      <c r="C26" t="inlineStr">
-        <is>
-          <t>Limonka szt              C</t>
-        </is>
-      </c>
-      <c r="D26" t="inlineStr">
-        <is>
-          <t>C</t>
-        </is>
-      </c>
-      <c r="E26" t="n">
-        <v>189</v>
-      </c>
-      <c r="F26" t="n">
-        <v>1134</v>
-      </c>
-      <c r="G26" t="inlineStr">
-        <is>
-          <t>6</t>
-        </is>
-      </c>
-      <c r="H26" t="inlineStr"/>
-      <c r="I26" t="inlineStr"/>
-      <c r="J26" t="inlineStr"/>
-      <c r="K26" t="inlineStr"/>
-      <c r="L26" t="inlineStr">
-        <is>
-          <t>Limonka szt</t>
-        </is>
-      </c>
-      <c r="M26" t="inlineStr"/>
-      <c r="N26" t="inlineStr"/>
-      <c r="O26" t="n">
-        <v>1134</v>
-      </c>
-      <c r="P26" t="n">
-        <v>11.34</v>
-      </c>
-    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>